<commit_message>
new resuslts (hw encoding)
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\encoding_bench\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032D5F81-5C76-4C4C-B926-C98EEF7D23EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D125971-36E2-4265-A39C-B7D1852FAE73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="13215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>video</t>
   </si>
@@ -42,9 +42,6 @@
     <t>encoded (SW)</t>
   </si>
   <si>
-    <t>time needed (SW)</t>
-  </si>
-  <si>
     <t>NBA</t>
   </si>
   <si>
@@ -70,6 +67,12 @@
   </si>
   <si>
     <t>duration vs encding time</t>
+  </si>
+  <si>
+    <t>SW</t>
+  </si>
+  <si>
+    <t>time needed(SW)</t>
   </si>
 </sst>
 </file>
@@ -100,7 +103,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -108,16 +111,102 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="45" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -399,172 +488,275 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="25.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
+    <col min="8" max="8" width="25.85546875" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="7"/>
+    </row>
+    <row r="2" spans="1:11" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>521.6</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3.2523148148148151E-3</v>
+      </c>
+      <c r="D3">
+        <v>192.2</v>
+      </c>
+      <c r="E3" s="3">
+        <f>(B3-D3)/B3</f>
+        <v>0.63151840490797551</v>
+      </c>
+      <c r="F3" s="2">
+        <v>6.1921296296296299E-3</v>
+      </c>
+      <c r="G3" s="3">
+        <f>F3/C3</f>
+        <v>1.9039145907473309</v>
+      </c>
+      <c r="H3">
+        <v>407.8</v>
+      </c>
+      <c r="I3" s="3">
+        <f t="shared" ref="I3:I5" si="0">($B3-H3)/B3</f>
+        <v>0.21817484662576689</v>
+      </c>
+      <c r="J3" s="2">
+        <v>3.9930555555555561E-3</v>
+      </c>
+      <c r="K3" s="3">
+        <f>J3/$C3</f>
+        <v>1.2277580071174379</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
+      <c r="B4">
+        <v>529.4</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3.0787037037037037E-3</v>
+      </c>
+      <c r="D4">
+        <v>200.8</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" ref="E4:E7" si="1">(B4-D4)/B4</f>
+        <v>0.62070268228182846</v>
+      </c>
+      <c r="F4" s="2">
+        <v>4.6180555555555558E-3</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" ref="G4:G7" si="2">F4/C4</f>
+        <v>1.5</v>
+      </c>
+      <c r="H4">
+        <v>351.2</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" si="0"/>
+        <v>0.33660748016622594</v>
+      </c>
+      <c r="J4" s="2">
+        <v>2.4421296296296296E-3</v>
+      </c>
+      <c r="K4" s="3">
+        <f t="shared" ref="K4:K7" si="3">J4/$C4</f>
+        <v>0.79323308270676696</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>521.6</v>
-      </c>
-      <c r="C2">
-        <v>192.2</v>
-      </c>
-      <c r="D2" s="3">
-        <f>(B2-C2)/B2</f>
-        <v>0.63151840490797551</v>
-      </c>
-      <c r="E2" s="2">
-        <v>3.2523148148148151E-3</v>
-      </c>
-      <c r="F2" s="2">
-        <v>6.1921296296296299E-3</v>
-      </c>
-      <c r="G2" s="3">
-        <f t="shared" ref="G2:G6" si="0">F2/E2</f>
-        <v>1.9039145907473309</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
-        <v>529.4</v>
-      </c>
-      <c r="C3">
-        <v>200.8</v>
-      </c>
-      <c r="D3" s="3">
-        <f t="shared" ref="D3:D6" si="1">(B3-C3)/B3</f>
-        <v>0.62070268228182846</v>
-      </c>
-      <c r="E3" s="2">
-        <v>3.0787037037037037E-3</v>
-      </c>
-      <c r="F3" s="2">
-        <v>4.6180555555555558E-3</v>
-      </c>
-      <c r="G3" s="3">
-        <f t="shared" si="0"/>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
+      <c r="B5">
         <v>1024</v>
       </c>
-      <c r="C4">
+      <c r="C5" s="2">
+        <v>3.6226851851851854E-3</v>
+      </c>
+      <c r="D5">
         <v>179.6</v>
       </c>
-      <c r="D4" s="3">
+      <c r="E5" s="3">
         <f t="shared" si="1"/>
         <v>0.82460937499999998</v>
       </c>
-      <c r="E4" s="2">
-        <v>3.6226851851851854E-3</v>
-      </c>
-      <c r="F4" s="2">
+      <c r="F5" s="2">
         <v>8.611111111111111E-3</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G5" s="3">
+        <f t="shared" si="2"/>
+        <v>2.3769968051118209</v>
+      </c>
+      <c r="H5">
+        <v>396.5</v>
+      </c>
+      <c r="I5" s="3">
         <f t="shared" si="0"/>
-        <v>2.3769968051118209</v>
+        <v>0.61279296875</v>
+      </c>
+      <c r="J5" s="2">
+        <v>6.2731481481481484E-3</v>
+      </c>
+      <c r="K5" s="3">
+        <f t="shared" si="3"/>
+        <v>1.7316293929712461</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
         <v>61.1</v>
       </c>
-      <c r="C5">
+      <c r="C6" s="2">
+        <v>3.3564814814814812E-4</v>
+      </c>
+      <c r="D6">
         <v>8.4</v>
       </c>
-      <c r="D5" s="3">
+      <c r="E6" s="3">
         <f t="shared" si="1"/>
         <v>0.86252045826513912</v>
       </c>
-      <c r="E5" s="2">
-        <v>3.3564814814814812E-4</v>
-      </c>
-      <c r="F5" s="2">
+      <c r="F6" s="2">
         <v>6.3657407407407402E-4</v>
       </c>
-      <c r="G5" s="3">
-        <f t="shared" si="0"/>
+      <c r="G6" s="3">
+        <f t="shared" si="2"/>
         <v>1.896551724137931</v>
       </c>
+      <c r="H6">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="I6" s="3">
+        <f>($B6-H6)/B6</f>
+        <v>0.69885433715220957</v>
+      </c>
+      <c r="J6" s="2">
+        <v>5.0925925925925921E-4</v>
+      </c>
+      <c r="K6" s="3">
+        <f t="shared" si="3"/>
+        <v>1.5172413793103448</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
         <v>441.2</v>
       </c>
-      <c r="C6">
+      <c r="C7" s="2">
+        <v>3.4027777777777784E-3</v>
+      </c>
+      <c r="D7">
         <v>179.4</v>
       </c>
-      <c r="D6" s="3">
+      <c r="E7" s="3">
         <f t="shared" si="1"/>
         <v>0.59338168631006338</v>
       </c>
-      <c r="E6" s="2">
-        <v>3.4027777777777784E-3</v>
-      </c>
-      <c r="F6" s="1">
+      <c r="F7" s="1">
         <v>4.8032407407407407E-3</v>
       </c>
-      <c r="G6" s="3">
-        <f t="shared" si="0"/>
+      <c r="G7" s="3">
+        <f t="shared" si="2"/>
         <v>1.4115646258503398</v>
+      </c>
+      <c r="H7">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="I7" s="3">
+        <f>($B7-H7)/B7</f>
+        <v>0.31233000906618319</v>
+      </c>
+      <c r="J7" s="2">
+        <v>2.1064814814814813E-3</v>
+      </c>
+      <c r="K7" s="3">
+        <f t="shared" si="3"/>
+        <v>0.61904761904761885</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="H1:K1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Minor fixes to script and excel file
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\encoding_bench\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documenti\Uni\compArch\encoding_bench\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D125971-36E2-4265-A39C-B7D1852FAE73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37ACCC5B-315D-45A6-BE0F-11D9ED7B0C1E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="13215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>video</t>
   </si>
@@ -66,13 +66,22 @@
     <t>duration</t>
   </si>
   <si>
-    <t>duration vs encding time</t>
-  </si>
-  <si>
     <t>SW</t>
   </si>
   <si>
     <t>time needed(SW)</t>
+  </si>
+  <si>
+    <t>duration vs encoding time</t>
+  </si>
+  <si>
+    <t>HW</t>
+  </si>
+  <si>
+    <t>time needed(HW)</t>
+  </si>
+  <si>
+    <t>encoded (HW)</t>
   </si>
 </sst>
 </file>
@@ -95,12 +104,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="7">
@@ -184,12 +199,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="45" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -201,12 +221,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="45" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -488,41 +505,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" customWidth="1"/>
-    <col min="8" max="8" width="25.85546875" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" customWidth="1"/>
+    <col min="9" max="9" width="11.5546875" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="7"/>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="8"/>
     </row>
-    <row r="2" spans="1:11" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -532,224 +550,224 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="8" t="s">
+      <c r="H2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="4" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>521.6</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>3.2523148148148151E-3</v>
       </c>
       <c r="D3">
         <v>192.2</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <f>(B3-D3)/B3</f>
         <v>0.63151840490797551</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>6.1921296296296299E-3</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <f>F3/C3</f>
         <v>1.9039145907473309</v>
       </c>
       <c r="H3">
         <v>407.8</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="2">
         <f t="shared" ref="I3:I5" si="0">($B3-H3)/B3</f>
         <v>0.21817484662576689</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="1">
         <v>3.9930555555555561E-3</v>
       </c>
-      <c r="K3" s="3">
+      <c r="K3" s="2">
         <f>J3/$C3</f>
         <v>1.2277580071174379</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
         <v>529.4</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>3.0787037037037037E-3</v>
       </c>
       <c r="D4">
         <v>200.8</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <f t="shared" ref="E4:E7" si="1">(B4-D4)/B4</f>
         <v>0.62070268228182846</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>4.6180555555555558E-3</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <f t="shared" ref="G4:G7" si="2">F4/C4</f>
         <v>1.5</v>
       </c>
       <c r="H4">
         <v>351.2</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="2">
         <f t="shared" si="0"/>
         <v>0.33660748016622594</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="1">
         <v>2.4421296296296296E-3</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="2">
         <f t="shared" ref="K4:K7" si="3">J4/$C4</f>
         <v>0.79323308270676696</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
         <v>1024</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>3.6226851851851854E-3</v>
       </c>
       <c r="D5">
         <v>179.6</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <f t="shared" si="1"/>
         <v>0.82460937499999998</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>8.611111111111111E-3</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <f t="shared" si="2"/>
         <v>2.3769968051118209</v>
       </c>
       <c r="H5">
         <v>396.5</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="2">
         <f t="shared" si="0"/>
         <v>0.61279296875</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="1">
         <v>6.2731481481481484E-3</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="2">
         <f t="shared" si="3"/>
         <v>1.7316293929712461</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>441.2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3.4027777777777784E-3</v>
+      </c>
+      <c r="D6">
+        <v>179.4</v>
+      </c>
+      <c r="E6" s="2">
+        <f>(B6-D6)/B6</f>
+        <v>0.59338168631006338</v>
+      </c>
+      <c r="F6" s="1">
+        <v>4.8032407407407407E-3</v>
+      </c>
+      <c r="G6" s="2">
+        <f>F6/C6</f>
+        <v>1.4115646258503398</v>
+      </c>
+      <c r="H6">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="I6" s="2">
+        <f>($B6-H6)/B6</f>
+        <v>0.31233000906618319</v>
+      </c>
+      <c r="J6" s="1">
+        <v>2.1064814814814813E-3</v>
+      </c>
+      <c r="K6" s="2">
+        <f>J6/$C6</f>
+        <v>0.61904761904761885</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="B8" s="9">
         <v>61.1</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C8" s="10">
         <v>3.3564814814814812E-4</v>
       </c>
-      <c r="D6">
+      <c r="D8" s="9">
         <v>8.4</v>
       </c>
-      <c r="E6" s="3">
-        <f t="shared" si="1"/>
+      <c r="E8" s="11">
+        <f>(B8-D8)/B8</f>
         <v>0.86252045826513912</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F8" s="10">
         <v>6.3657407407407402E-4</v>
       </c>
-      <c r="G6" s="3">
-        <f t="shared" si="2"/>
+      <c r="G8" s="11">
+        <f>F8/C8</f>
         <v>1.896551724137931</v>
       </c>
-      <c r="H6">
+      <c r="H8" s="9">
         <v>18.399999999999999</v>
       </c>
-      <c r="I6" s="3">
-        <f>($B6-H6)/B6</f>
+      <c r="I8" s="11">
+        <f>($B8-H8)/B8</f>
         <v>0.69885433715220957</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J8" s="10">
         <v>5.0925925925925921E-4</v>
       </c>
-      <c r="K6" s="3">
-        <f t="shared" si="3"/>
+      <c r="K8" s="11">
+        <f>J8/$C8</f>
         <v>1.5172413793103448</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>441.2</v>
-      </c>
-      <c r="C7" s="2">
-        <v>3.4027777777777784E-3</v>
-      </c>
-      <c r="D7">
-        <v>179.4</v>
-      </c>
-      <c r="E7" s="3">
-        <f t="shared" si="1"/>
-        <v>0.59338168631006338</v>
-      </c>
-      <c r="F7" s="1">
-        <v>4.8032407407407407E-3</v>
-      </c>
-      <c r="G7" s="3">
-        <f t="shared" si="2"/>
-        <v>1.4115646258503398</v>
-      </c>
-      <c r="H7">
-        <v>303.39999999999998</v>
-      </c>
-      <c r="I7" s="3">
-        <f>($B7-H7)/B7</f>
-        <v>0.31233000906618319</v>
-      </c>
-      <c r="J7" s="2">
-        <v>2.1064814814814813E-3</v>
-      </c>
-      <c r="K7" s="3">
-        <f t="shared" si="3"/>
-        <v>0.61904761904761885</v>
       </c>
     </row>
   </sheetData>

</xml_diff>